<commit_message>
Finish PostProcessing with VBA
</commit_message>
<xml_diff>
--- a/6. Results/Results.xlsx
+++ b/6. Results/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\monty.minh\Documents\Optimizer\6. Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009FDC80-104E-4FDD-A67E-EF14D2713340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C0C4E0-558D-49BD-B5E4-E606976B5808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1131" yWindow="1131" windowWidth="10578" windowHeight="4946" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10660" yWindow="-21710" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inbound Cost Per Factory" sheetId="1" r:id="rId1"/>
@@ -18,24 +18,12 @@
     <sheet name="Inbound Volume Per Factory" sheetId="3" r:id="rId3"/>
     <sheet name="Outbound Volume Per Customer" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="13">
   <si>
     <t>Factory</t>
   </si>
@@ -43,10 +31,10 @@
     <t>Product</t>
   </si>
   <si>
+    <t>Binh Dinh</t>
+  </si>
+  <si>
     <t>Hai Phong</t>
-  </si>
-  <si>
-    <t>Binh Dinh</t>
   </si>
   <si>
     <t>Bag</t>
@@ -475,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -505,10 +493,10 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>666.66666666666674</v>
+        <v>600</v>
       </c>
       <c r="D2">
-        <v>360</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -516,13 +504,27 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>300</v>
+      </c>
+      <c r="D3">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>2437.5</v>
-      </c>
-      <c r="D3">
-        <v>2790</v>
+      <c r="C4">
+        <v>1350</v>
+      </c>
+      <c r="D4">
+        <v>1530</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>600</v>
@@ -589,7 +591,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>400</v>
@@ -609,7 +611,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>900</v>
@@ -629,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>1200</v>
@@ -649,7 +651,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>1050</v>
@@ -665,11 +667,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -695,10 +695,10 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>16.666666666666671</v>
+        <v>20</v>
       </c>
       <c r="D2">
-        <v>12</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
@@ -706,13 +706,27 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>81.25</v>
-      </c>
-      <c r="D3">
-        <v>93</v>
+      <c r="C4">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -724,9 +738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
@@ -761,7 +773,7 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -781,7 +793,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -801,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -821,7 +833,7 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5">
         <v>20</v>
@@ -841,7 +853,7 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E6">
         <v>15</v>

</xml_diff>